<commit_message>
Fixed for Cross entropy log loss for binary OHE cases.
</commit_message>
<xml_diff>
--- a/nlp/src/common/cross_entropy_log_loss_input_combinations.xlsx
+++ b/nlp/src/common/cross_entropy_log_loss_input_combinations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/237ac6b38ade988b/Documents/Technologies/GA/ML/notes/NN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="592" documentId="8_{59FB4E2D-B7D2-4154-BE6F-07FF7F6B7527}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A4B124BC-B122-4FF5-80BB-3322BCF524A5}"/>
+  <xr:revisionPtr revIDLastSave="690" documentId="8_{59FB4E2D-B7D2-4154-BE6F-07FF7F6B7527}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{30D1C2E6-FB14-41E3-A163-4D54C1D58900}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{98ED04F0-3849-4411-9D14-68882DBC6643}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{98ED04F0-3849-4411-9D14-68882DBC6643}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$A$1:$D$13</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
   <si>
     <t>P</t>
   </si>
@@ -697,23 +698,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>N</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">T is binary label 0/1
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Return -T * log(P)</t>
     </r>
   </si>
   <si>
@@ -899,35 +883,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">T is index label
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>P.ndim=1 and T.ndim=0 and (P.shape != T.shape)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-* T=1 for P[0.9]
-* T=2 for P[0.0, 0.1,0.9]</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>P:ndarray(</t>
     </r>
     <r>
@@ -1392,72 +1347,549 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">DO NOT P.reshape((1, -1))
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">T = np.argmax(T) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and T.reshape(-1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+T.reshape(N) enforces 1D array for T and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>np.argmax(T) result in () when T:(M,)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+No need to np.array(T) becuause other than P:scalar and T:scalar, P and T must be ndarray. It must be assured before.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">T is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>binary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OHE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> label 0/1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Return -T * log(P)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">P.ndim=1 and T.ndim=0 and (P.shape != T.shape)
+- Binary OHE label when M=1 (M is size of P in 1D or P.shape[0])
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">e.g. T=1 for P[0.9]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Transfoer to (P.ndim=0, T.ndim=0)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> state.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">np.array(T).reshape(())
+np.array(P).reshape(())
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Index label when M&gt;1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">e.g. T=2 for P[0.0, 0.1,0.9]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Transfer to (P.ndim=2, T.ndim=1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> state
+np.array(T).reshape(-1)
+np.array(P).reshape(1, -1)</t>
+    </r>
+  </si>
+  <si>
+    <t>BEFORE</t>
+  </si>
+  <si>
+    <t>AFTER</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(P:spahe == T.shape == M) and (P.ndim == T.ndim ==1) and (P.size == T.size == M)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Binary OHE label when M=1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">e.g. T[1] for P[1.0] 
+Transfer to (P.ndim=0, T.ndim=0) state.
+np.array(T).reshape(())
+np.array(P).reshape(())
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Index label when M&gt;1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e.g. T[0,0,1] for P[0., 0., 1.] 
+Transfer to (P.ndim=2, T.ndim=1) state
+np.array(T).reshape(-1)
+np.array(P).reshape(1, -1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">T is OHE label
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(P:spahe == T.shape ==N) and (P.ndim == T.ndim ==2) and P.size = T.size == N*M)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-* T[
+(P:spahe == T.shape ==N) and (P.ndim == T.ndim ==2) and P.size = T.size == N*M)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Binary OHE label when M=1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">e.g. T[
+   [0],[1],[0]
+]
+P[
+   [0.9],[0.1],[0.3]
+]
+Stay here
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Index label when M&gt;1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e.g. T[
   [0,0,1,0],
   [0,1,0,0]
 ] for P[
   [0., 0., 0.99, 0.]
   [0., 1., 0., 0.]
+]
+Transfer to (P.ndim=2, T.ndim=1) state
+np.array(T).reshape(-1)
+np.array(P).reshape(1, -1)
 ]</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">T is OHE label.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(P:spahe == T.shape == M) and (P.ndim == T.ndim ==1) and (P.size == T.size == M)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+      <t xml:space="preserve">T is index label
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(P.shape[0] == T.shape[0] ==N) and
+(P.ndim == T.ndim+1)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NOT alwasys (P.size == T.size)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-* T[1] for P[1.0] 
-* T[0,0,1] for P[0., 0., 1.] </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">T is index label
-</t>
-    </r>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Index label when M&gt;1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+e.g. T [0,1,0,0]
+P[
+  [0., 0., 0.99, 0.],
+  [0., 1., 0., 0.],
+  [0., 1., 0., 0.],
+  [0., 1., 0., 0.]
+]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">T is binary OHE label
+(1 &lt; P.ndim == T.ndim) and 
+(P:spahe[1] == T.shape[1] == 1) and 
+(P.size = T.size) and 
+np.all(T &lt;=1) == True
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Binary OHE label and M=1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">e.g. T[
+   [0],[1],[0]
+]
+P[
+   [0.9],[0.1],[0.3]
+]
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">T is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>binary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OHE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> label 0/1
+P.ndim == T.ndim == 0
+(T &lt;=1) == True
+e.g. T=0, P=0.9
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Return -T * log(P)</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -1500,46 +1932,59 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">* T[0, 1] for P[
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Binary OHE label when M=1  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">must np.all(T &lt;=1) == True
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">e.g. T[0, 1] for P[
   [0.0], 
   [1.0]  
 ]
-* </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">DO NOT P.reshape((1, -1))
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">T = np.argmax(T) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and T.reshape(-1)</t>
+Transfer to (P.ndim=2, T.ndim=2) state
+T.reshape(-1, 1)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Index label when M&gt;1</t>
     </r>
     <r>
       <rPr>
@@ -1550,29 +1995,14 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-T.reshape(N) enforces 1D array for T and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>np.argmax(T) result in () when T:(M,)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-No need to np.array(T) becuause other than P:scalar and T:scalar, P and T must be ndarray. It must be assured before.</t>
+e.g. T [0,1,0,0]
+P[
+  [0., 0., 0.99, 0.],
+  [0., 1., 0., 0.],
+  [0., 1., 0., 0.],
+  [0., 1., 0., 0.]
+]
+Stay here.</t>
     </r>
   </si>
 </sst>
@@ -1580,7 +2010,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1651,6 +2081,22 @@
     <font>
       <sz val="11"/>
       <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1906,7 +2352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1956,15 +2402,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1974,8 +2414,14 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2033,6 +2479,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2351,7 +2806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D017FF-AABD-4984-89E0-889D2C86F474}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -2533,13 +2988,13 @@
         <v>36</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>42</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2547,10 +3002,10 @@
         <v>22</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="27"/>
       <c r="E15" s="8"/>
@@ -2609,7 +3064,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
@@ -2618,16 +3073,16 @@
     </row>
     <row r="21" spans="1:5" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="C21" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>59</v>
-      </c>
       <c r="D21" s="24" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>14</v>
@@ -2641,7 +3096,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D22" s="25"/>
       <c r="E22" s="7" t="s">
@@ -2656,7 +3111,7 @@
         <v>17</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D23" s="25"/>
       <c r="E23" s="7" t="s">
@@ -2682,9 +3137,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA661ADB-2504-4897-AD75-6CCA76B56DE2}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2692,72 +3147,163 @@
   <cols>
     <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.88671875" customWidth="1"/>
-    <col min="3" max="3" width="51.44140625" customWidth="1"/>
-    <col min="4" max="4" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="54.77734375" customWidth="1"/>
+    <col min="4" max="4" width="51.21875" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="50.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+      <c r="B1" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="45" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B3" s="22">
         <v>0</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C3" s="22">
         <v>1</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D3" s="22">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18">
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17">
         <v>0</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="20" t="s">
+      <c r="B4" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D4" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="121.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18">
+    <row r="5" spans="1:4" ht="222" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17">
         <v>1</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="20" t="s">
+      <c r="B5" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="152.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18">
+    <row r="6" spans="1:4" ht="360" x14ac:dyDescent="0.3">
+      <c r="A6" s="17">
         <v>2</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C6" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="21" t="s">
-        <v>62</v>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="22">
+        <v>0</v>
+      </c>
+      <c r="C10" s="22">
+        <v>1</v>
+      </c>
+      <c r="D10" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="17">
+        <v>0</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17">
+        <v>1</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="17">
+        <v>2</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <mergeCells count="4">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="46" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>